<commit_message>
Comentado e Organizado pt.1
</commit_message>
<xml_diff>
--- a/Resultados/Material + Ano + Estrutura/ResNet/Tentativa 1/Com Tentativa 1 - Material + Ano (Com Tentativa 1 - Material).xlsx
+++ b/Resultados/Material + Ano + Estrutura/ResNet/Tentativa 1/Com Tentativa 1 - Material + Ano (Com Tentativa 1 - Material).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="EsteLivro" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beatr\Documents\GitHub\SAFENET-Bea\Resultados\Material + Ano + Estrutura\ResNet\Tentativa 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B304D6D-2959-4B17-9C2B-B322AD4488D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30416B9D-3157-4B70-89F2-AAC0D7D39D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{44EB1693-29A4-4AD6-9832-A8AEAD2DC94E}"/>
   </bookViews>
@@ -597,6 +597,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -605,9 +608,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -618,8 +618,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -627,6 +627,95 @@
     <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -721,95 +810,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1300,23 +1300,23 @@
   <autoFilter ref="A1:J12" xr:uid="{05CD79ED-E271-418B-AE5D-0CEC67D117D8}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{0BC8D92E-F05A-4765-ADE7-158957752698}" name="Classe" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{158B1DC5-8A42-4E97-A9C4-3F00630EA162}" name="Accuracy" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{C65D27B5-BF2B-480F-9245-88EBC462C418}" name="Precision" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{2F039AB7-CAFE-4D33-8E3F-DDB0554402B9}" name="Recall" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{E8A788D3-B0FB-4153-AC29-EB77EB842308}" name="F1 Score" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{76122F43-3076-419C-936F-1BAB3AB79795}" name="Qtd" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{158B1DC5-8A42-4E97-A9C4-3F00630EA162}" name="Accuracy" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C65D27B5-BF2B-480F-9245-88EBC462C418}" name="Precision" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{2F039AB7-CAFE-4D33-8E3F-DDB0554402B9}" name="Recall" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{E8A788D3-B0FB-4153-AC29-EB77EB842308}" name="F1 Score" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{76122F43-3076-419C-936F-1BAB3AB79795}" name="Qtd" dataDxfId="4">
       <calculatedColumnFormula>'Matriz Confusão 2'!N3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{ED69C583-BA02-4717-B168-089B7EA09073}" name="Exatidão" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{ED69C583-BA02-4717-B168-089B7EA09073}" name="Exatidão" dataDxfId="3">
       <calculatedColumnFormula array="1">_xlfn.IFS(AND(B2&lt;=1,B2&gt;=0.95),"Muito Alta",AND(B2&lt;0.95,B2&gt;=0.9),"Alta",AND(B2&lt;0.9,B2&gt;=0.7),"Boa",AND(B2&lt;0.7,B2&gt;=0.5),"Médio",AND(B2&lt;0.5,B2&gt;=0.25),"Baixo",AND(B2&lt;0.25,B2&gt;0),"Muito Baixo",B2=0,"Zero")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{52506CAA-318D-400D-AA3D-9DD38E4BE67E}" name="Precisão" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{52506CAA-318D-400D-AA3D-9DD38E4BE67E}" name="Precisão" dataDxfId="2">
       <calculatedColumnFormula array="1">_xlfn.IFS(AND(C2&lt;=1,C2&gt;=0.95),"Muito Alta",AND(C2&lt;0.95,C2&gt;=0.9),"Alta",AND(C2&lt;0.9,C2&gt;=0.7),"Boa",AND(C2&lt;0.7,C2&gt;=0.5),"Médio",AND(C2&lt;0.5,C2&gt;=0.25),"Baixo",AND(C2&lt;0.25,C2&gt;0),"Muito Baixo",C2=0,"Zero")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{80EB9D07-1FE1-4C36-89EB-4BFB293D3A96}" name="Recuperação" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{80EB9D07-1FE1-4C36-89EB-4BFB293D3A96}" name="Recuperação" dataDxfId="1">
       <calculatedColumnFormula array="1">_xlfn.IFS(AND(D2&lt;=1,D2&gt;=0.95),"Muito Alta",AND(D2&lt;0.95,D2&gt;=0.9),"Alta",AND(D2&lt;0.9,D2&gt;=0.7),"Boa",AND(D2&lt;0.7,D2&gt;=0.5),"Médio",AND(D2&lt;0.5,D2&gt;=0.25),"Baixo",AND(D2&lt;0.25,D2&gt;0),"Muito Baixo",D2=0,"Zero")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3B26B576-C152-418D-BC1D-A627F1BEAA9C}" name="F1" dataDxfId="4">
+    <tableColumn id="10" xr3:uid="{3B26B576-C152-418D-BC1D-A627F1BEAA9C}" name="F1" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn.IFS(AND(E2&lt;=1,E2&gt;=0.95),"Muito Alta",AND(E2&lt;0.95,E2&gt;=0.9),"Alta",AND(E2&lt;0.9,E2&gt;=0.7),"Boa",AND(E2&lt;0.7,E2&gt;=0.5),"Médio",AND(E2&lt;0.5,E2&gt;=0.25),"Baixo",AND(E2&lt;0.25,E2&gt;0),"Muito Baixo",E2=0,"Zero")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1644,8 +1644,8 @@
   <sheetPr codeName="Folha1"/>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1845,23 +1845,23 @@
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="50">
+      <c r="B12" s="51">
         <v>0.80864077806472701</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="50">
+      <c r="B13" s="51">
         <v>0.801857590675354</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
@@ -1978,8 +1978,8 @@
   <sheetPr codeName="Folha12"/>
   <dimension ref="N1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2256,7 +2256,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N14"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2267,19 +2267,19 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1"/>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2"/>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52" t="str">
+      <c r="A3" s="53" t="str">
         <f>"Verdadeiro"</f>
         <v>Verdadeiro</v>
       </c>
@@ -2367,7 +2367,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -2413,7 +2413,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="52"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -2505,7 +2505,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="52"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -2551,7 +2551,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="52"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -2597,7 +2597,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -2643,7 +2643,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="52"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -2689,7 +2689,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -2735,7 +2735,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="52"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="1">
         <v>9</v>
       </c>
@@ -2781,7 +2781,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="52"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="1">
         <v>10</v>
       </c>
@@ -2892,9 +2892,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB454C8-93BE-43D4-99C2-717E269EE6C9}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P30" sqref="P30"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2903,7 +2903,7 @@
     <col min="2" max="2" width="10.6328125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.453125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.36328125" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.26953125" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="26" bestFit="1" customWidth="1"/>
@@ -2912,7 +2912,7 @@
     <col min="11" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.54296875" customWidth="1"/>
+    <col min="14" max="14" width="4.36328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.6328125" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
@@ -2971,12 +2971,12 @@
       <c r="V1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="53" t="s">
+      <c r="X1" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
     </row>
     <row r="2" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="54" t="s">
@@ -3118,7 +3118,7 @@
         <v>26</v>
       </c>
       <c r="X3" s="18">
-        <f>COUNTIF($D:$D,Y3)+COUNTIF($M:$M,Y3)</f>
+        <f t="shared" ref="X3:X9" si="6">COUNTIF($D:$D,Y3)+COUNTIF($M:$M,Y3)</f>
         <v>9</v>
       </c>
       <c r="Y3" s="21" t="s">
@@ -3138,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="21" t="str">
-        <f t="shared" ref="D4:D5" si="6">COUNTIF(F4,$F$2)+COUNTIF(G4,$G$2)+COUNTIF(H4,$H$2)&amp;" ("&amp; IF(F4=$F$2,"Estrutura, ","") &amp; IF(G4=$G$2,"Ano, ","") &amp;IF(H4=$H$2,"Material","") &amp; IF(OR(F4=$F$2,G4=$G$2,H4=$H$2),"","Nenhuma") &amp;")"</f>
+        <f t="shared" ref="D4:D5" si="7">COUNTIF(F4,$F$2)+COUNTIF(G4,$G$2)+COUNTIF(H4,$H$2)&amp;" ("&amp; IF(F4=$F$2,"Estrutura, ","") &amp; IF(G4=$G$2,"Ano, ","") &amp;IF(H4=$H$2,"Material","") &amp; IF(OR(F4=$F$2,G4=$G$2,H4=$H$2),"","Nenhuma") &amp;")"</f>
         <v>0 (Nenhuma)</v>
       </c>
       <c r="E4" s="47">
@@ -3165,7 +3165,7 @@
         <v>5</v>
       </c>
       <c r="M4" s="21" t="str">
-        <f t="shared" ref="M4:M6" si="7">COUNTIF(O4,$O$2)+COUNTIF(P4,$P$2)+COUNTIF(Q4,$Q$2)&amp;" ("&amp; IF(O4=$O$2,"Estrutura, ","") &amp; IF(P4=$P$2,"Ano, ","") &amp;IF(Q4=$Q$2,"Material","") &amp; IF(OR(O4=$O$2,P4=$P$2,Q4=$Q$2),"","Nenhuma") &amp;")"</f>
+        <f t="shared" ref="M4:M6" si="8">COUNTIF(O4,$O$2)+COUNTIF(P4,$P$2)+COUNTIF(Q4,$Q$2)&amp;" ("&amp; IF(O4=$O$2,"Estrutura, ","") &amp; IF(P4=$P$2,"Ano, ","") &amp;IF(Q4=$Q$2,"Material","") &amp; IF(OR(O4=$O$2,P4=$P$2,Q4=$Q$2),"","Nenhuma") &amp;")"</f>
         <v>2 (Estrutura, Material)</v>
       </c>
       <c r="N4" s="47">
@@ -3173,15 +3173,15 @@
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="O4" s="26" t="str">
-        <f t="shared" ref="O4:O6" si="8">VLOOKUP(L4,$S$1:$V$12,2,FALSE)</f>
+        <f t="shared" ref="O4:O6" si="9">VLOOKUP(L4,$S$1:$V$12,2,FALSE)</f>
         <v>Pórtico</v>
       </c>
       <c r="P4" s="26" t="str">
-        <f t="shared" ref="P4:P6" si="9">VLOOKUP(L4,$S$1:$V$12,3,FALSE)</f>
+        <f t="shared" ref="P4:P6" si="10">VLOOKUP(L4,$S$1:$V$12,3,FALSE)</f>
         <v>Antes de 1983</v>
       </c>
       <c r="Q4" s="26" t="str">
-        <f t="shared" ref="Q4:Q6" si="10">VLOOKUP(L4,$S$1:$V$12,4,FALSE)</f>
+        <f t="shared" ref="Q4:Q6" si="11">VLOOKUP(L4,$S$1:$V$12,4,FALSE)</f>
         <v>Betão Armado</v>
       </c>
       <c r="S4" s="18">
@@ -3195,14 +3195,14 @@
         <v>26</v>
       </c>
       <c r="X4" s="18">
-        <f>COUNTIF($D:$D,Y4)+COUNTIF($M:$M,Y4)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y4" s="21" t="s">
         <v>50</v>
       </c>
       <c r="Z4" s="42">
-        <f t="shared" ref="Z4:Z9" si="11">X4/$X$10</f>
+        <f t="shared" ref="Z4:Z9" si="12">X4/$X$10</f>
         <v>0</v>
       </c>
     </row>
@@ -3215,7 +3215,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0 (Nenhuma)</v>
       </c>
       <c r="E5" s="47">
@@ -3242,7 +3242,7 @@
         <v>7</v>
       </c>
       <c r="M5" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1 (Material)</v>
       </c>
       <c r="N5" s="47">
@@ -3250,15 +3250,15 @@
         <v>4.6296296296296294E-2</v>
       </c>
       <c r="O5" s="26" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Tabuleiro simples/apoiado</v>
       </c>
       <c r="P5" s="26" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Antes de 1983</v>
       </c>
       <c r="Q5" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Betão Armado</v>
       </c>
       <c r="S5" s="18">
@@ -3274,14 +3274,14 @@
         <v>25</v>
       </c>
       <c r="X5" s="18">
-        <f>COUNTIF($D:$D,Y5)+COUNTIF($M:$M,Y5)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="Y5" s="21" t="s">
         <v>39</v>
       </c>
       <c r="Z5" s="42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -3300,7 +3300,7 @@
         <v>10</v>
       </c>
       <c r="M6" s="21" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2 (Ano, Material)</v>
       </c>
       <c r="N6" s="47">
@@ -3308,15 +3308,15 @@
         <v>6.4814814814814811E-2</v>
       </c>
       <c r="O6" s="26" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Vãos Multiplos</v>
       </c>
       <c r="P6" s="26" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Depois de 1983</v>
       </c>
       <c r="Q6" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>Betão Armado</v>
       </c>
       <c r="S6" s="18">
@@ -3332,14 +3332,14 @@
         <v>25</v>
       </c>
       <c r="X6" s="18">
-        <f>COUNTIF($D:$D,Y6)+COUNTIF($M:$M,Y6)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="Y6" s="21" t="s">
         <v>51</v>
       </c>
       <c r="Z6" s="42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.21875</v>
       </c>
     </row>
@@ -3382,14 +3382,14 @@
         <v>25</v>
       </c>
       <c r="X7" s="18">
-        <f>COUNTIF($D:$D,Y7)+COUNTIF($M:$M,Y7)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y7" s="21" t="s">
         <v>52</v>
       </c>
       <c r="Z7" s="42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -3436,15 +3436,15 @@
       </c>
       <c r="N8" s="40"/>
       <c r="O8" s="25" t="str">
-        <f t="shared" ref="O8:O12" si="12">VLOOKUP(L8,$S$1:$V$12,2,FALSE)</f>
+        <f t="shared" ref="O8:O12" si="13">VLOOKUP(L8,$S$1:$V$12,2,FALSE)</f>
         <v>Tabuleiro simples/apoiado</v>
       </c>
       <c r="P8" s="25" t="str">
-        <f t="shared" ref="P8:P12" si="13">VLOOKUP(L8,$S$1:$V$12,3,FALSE)</f>
+        <f t="shared" ref="P8:P12" si="14">VLOOKUP(L8,$S$1:$V$12,3,FALSE)</f>
         <v>Antes de 1983</v>
       </c>
       <c r="Q8" s="25" t="str">
-        <f t="shared" ref="Q8:Q12" si="14">VLOOKUP(L8,$S$1:$V$12,4,FALSE)</f>
+        <f t="shared" ref="Q8:Q12" si="15">VLOOKUP(L8,$S$1:$V$12,4,FALSE)</f>
         <v>Betão Armado</v>
       </c>
       <c r="S8" s="18">
@@ -3460,14 +3460,14 @@
         <v>25</v>
       </c>
       <c r="X8" s="18">
-        <f>COUNTIF($D:$D,Y8)+COUNTIF($M:$M,Y8)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="Y8" s="21" t="s">
         <v>53</v>
       </c>
       <c r="Z8" s="42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.15625</v>
       </c>
     </row>
@@ -3488,15 +3488,15 @@
         <v>0.05</v>
       </c>
       <c r="O9" s="26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P9" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q9" s="26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Alvenaria</v>
       </c>
       <c r="S9" s="18">
@@ -3512,14 +3512,14 @@
         <v>25</v>
       </c>
       <c r="X9" s="18">
-        <f>COUNTIF($D:$D,Y9)+COUNTIF($M:$M,Y9)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="Y9" s="21" t="s">
         <v>54</v>
       </c>
       <c r="Z9" s="42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.28125</v>
       </c>
     </row>
@@ -3565,15 +3565,15 @@
         <v>0.1</v>
       </c>
       <c r="O10" s="26" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Pórtico</v>
       </c>
       <c r="P10" s="26" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Depois de 1983</v>
       </c>
       <c r="Q10" s="26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Betão Armado</v>
       </c>
       <c r="S10" s="18">
@@ -3637,15 +3637,15 @@
         <v>0.05</v>
       </c>
       <c r="O11" s="26" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Tabuleiro simples/apoiado</v>
       </c>
       <c r="P11" s="26" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Depois de 1983</v>
       </c>
       <c r="Q11" s="26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Betão Armado</v>
       </c>
       <c r="S11" s="18">
@@ -3678,15 +3678,15 @@
         <v>0.25</v>
       </c>
       <c r="O12" s="26" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>Vãos Multiplos</v>
       </c>
       <c r="P12" s="26" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Depois de 1983</v>
       </c>
       <c r="Q12" s="26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Betão Armado</v>
       </c>
       <c r="S12" s="18">
@@ -3718,15 +3718,15 @@
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="25" t="str">
-        <f t="shared" ref="F13:F16" si="15">VLOOKUP(C13,$S$1:$V$12,2,FALSE)</f>
+        <f t="shared" ref="F13:F16" si="16">VLOOKUP(C13,$S$1:$V$12,2,FALSE)</f>
         <v>Arco</v>
       </c>
       <c r="G13" s="25" t="str">
-        <f t="shared" ref="G13:G16" si="16">VLOOKUP(C13,$S$1:$V$12,3,FALSE)</f>
+        <f t="shared" ref="G13:G16" si="17">VLOOKUP(C13,$S$1:$V$12,3,FALSE)</f>
         <v>Antes de 1983</v>
       </c>
       <c r="H13" s="25" t="str">
-        <f t="shared" ref="H13:H16" si="17">VLOOKUP(C13,$S$1:$V$12,4,FALSE)</f>
+        <f t="shared" ref="H13:H16" si="18">VLOOKUP(C13,$S$1:$V$12,4,FALSE)</f>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -3747,15 +3747,15 @@
         <v>0.2</v>
       </c>
       <c r="F14" s="26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G14" s="26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H14" s="26" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Alvenaria</v>
       </c>
       <c r="J14" s="54" t="s">
@@ -3777,11 +3777,11 @@
         <v>Tabuleiro simples/apoiado</v>
       </c>
       <c r="P14" s="25" t="str">
-        <f t="shared" ref="P14:P18" si="18">VLOOKUP(L14,$S$1:$V$12,3,FALSE)</f>
+        <f t="shared" ref="P14:P18" si="19">VLOOKUP(L14,$S$1:$V$12,3,FALSE)</f>
         <v>Depois de 1983</v>
       </c>
       <c r="Q14" s="25" t="str">
-        <f t="shared" ref="Q14:Q18" si="19">VLOOKUP(L14,$S$1:$V$12,4,FALSE)</f>
+        <f t="shared" ref="Q14:Q18" si="20">VLOOKUP(L14,$S$1:$V$12,4,FALSE)</f>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -3802,15 +3802,15 @@
         <v>0.2</v>
       </c>
       <c r="F15" s="26" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Tabuleiro simples/apoiado</v>
       </c>
       <c r="G15" s="26" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Antes de 1983</v>
       </c>
       <c r="H15" s="26" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Betão Armado</v>
       </c>
       <c r="J15" s="55"/>
@@ -3833,11 +3833,11 @@
         <v>0</v>
       </c>
       <c r="P15" s="26">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q15" s="26" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Alvenaria</v>
       </c>
     </row>
@@ -3858,15 +3858,15 @@
         <v>0.2</v>
       </c>
       <c r="F16" s="26" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Vãos Multiplos</v>
       </c>
       <c r="G16" s="26" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Depois de 1983</v>
       </c>
       <c r="H16" s="26" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Betão Armado</v>
       </c>
       <c r="J16" s="55"/>
@@ -3881,19 +3881,19 @@
         <v>2 (Ano, Material)</v>
       </c>
       <c r="N16" s="47">
-        <f t="shared" ref="N16:N18" si="20">K16/SUM(K15:K19)</f>
+        <f t="shared" ref="N16:N18" si="21">K16/SUM(K15:K19)</f>
         <v>0.32142857142857145</v>
       </c>
       <c r="O16" s="26" t="str">
-        <f t="shared" ref="O16:O18" si="21">VLOOKUP(L16,$S$1:$V$12,2,FALSE)</f>
+        <f t="shared" ref="O16:O18" si="22">VLOOKUP(L16,$S$1:$V$12,2,FALSE)</f>
         <v>Pórtico</v>
       </c>
       <c r="P16" s="26" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>Depois de 1983</v>
       </c>
       <c r="Q16" s="26" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -3910,24 +3910,24 @@
         <v>2 (Estrutura, Material)</v>
       </c>
       <c r="N17" s="47">
+        <f t="shared" si="21"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="O17" s="26" t="str">
+        <f t="shared" si="22"/>
+        <v>Tabuleiro simples/apoiado</v>
+      </c>
+      <c r="P17" s="26" t="str">
+        <f t="shared" si="19"/>
+        <v>Antes de 1983</v>
+      </c>
+      <c r="Q17" s="26" t="str">
         <f t="shared" si="20"/>
-        <v>7.407407407407407E-2</v>
-      </c>
-      <c r="O17" s="26" t="str">
-        <f t="shared" si="21"/>
-        <v>Tabuleiro simples/apoiado</v>
-      </c>
-      <c r="P17" s="26" t="str">
-        <f t="shared" si="18"/>
-        <v>Antes de 1983</v>
-      </c>
-      <c r="Q17" s="26" t="str">
-        <f t="shared" si="19"/>
         <v>Betão Armado</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="50" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="22">
@@ -3965,19 +3965,19 @@
         <v>2 (Ano, Material)</v>
       </c>
       <c r="N18" s="47">
+        <f t="shared" si="21"/>
+        <v>0.84210526315789469</v>
+      </c>
+      <c r="O18" s="26" t="str">
+        <f t="shared" si="22"/>
+        <v>Vãos Multiplos</v>
+      </c>
+      <c r="P18" s="26" t="str">
+        <f t="shared" si="19"/>
+        <v>Depois de 1983</v>
+      </c>
+      <c r="Q18" s="26" t="str">
         <f t="shared" si="20"/>
-        <v>0.84210526315789469</v>
-      </c>
-      <c r="O18" s="26" t="str">
-        <f t="shared" si="21"/>
-        <v>Vãos Multiplos</v>
-      </c>
-      <c r="P18" s="26" t="str">
-        <f t="shared" si="18"/>
-        <v>Depois de 1983</v>
-      </c>
-      <c r="Q18" s="26" t="str">
-        <f t="shared" si="19"/>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -3997,15 +3997,15 @@
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="25" t="str">
-        <f t="shared" ref="F20:F24" si="22">VLOOKUP(C20,$S$1:$V$12,2,FALSE)</f>
+        <f t="shared" ref="F20:F24" si="23">VLOOKUP(C20,$S$1:$V$12,2,FALSE)</f>
         <v>Pórtico</v>
       </c>
       <c r="G20" s="25" t="str">
-        <f t="shared" ref="G20:G24" si="23">VLOOKUP(C20,$S$1:$V$12,3,FALSE)</f>
+        <f t="shared" ref="G20:G24" si="24">VLOOKUP(C20,$S$1:$V$12,3,FALSE)</f>
         <v>Antes de 1983</v>
       </c>
       <c r="H20" s="25" t="str">
-        <f t="shared" ref="H20:H24" si="24">VLOOKUP(C20,$S$1:$V$12,4,FALSE)</f>
+        <f t="shared" ref="H20:H24" si="25">VLOOKUP(C20,$S$1:$V$12,4,FALSE)</f>
         <v>Betão Armado</v>
       </c>
       <c r="J20" s="54" t="s">
@@ -4027,11 +4027,11 @@
         <v>Vãos Multiplos</v>
       </c>
       <c r="P20" s="25" t="str">
-        <f t="shared" ref="P20:P24" si="25">VLOOKUP(L20,$S$1:$V$12,3,FALSE)</f>
+        <f t="shared" ref="P20:P24" si="26">VLOOKUP(L20,$S$1:$V$12,3,FALSE)</f>
         <v>Antes de 1983</v>
       </c>
       <c r="Q20" s="25" t="str">
-        <f t="shared" ref="Q20:Q24" si="26">VLOOKUP(L20,$S$1:$V$12,4,FALSE)</f>
+        <f t="shared" ref="Q20:Q24" si="27">VLOOKUP(L20,$S$1:$V$12,4,FALSE)</f>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -4052,15 +4052,15 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="F21" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="G21" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H21" s="26" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Alvenaria</v>
       </c>
       <c r="J21" s="55"/>
@@ -4083,11 +4083,11 @@
         <v>0</v>
       </c>
       <c r="P21" s="26" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>Antes de 1983</v>
       </c>
       <c r="Q21" s="26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>Aço</v>
       </c>
     </row>
@@ -4108,15 +4108,15 @@
         <v>0.45454545454545453</v>
       </c>
       <c r="F22" s="26" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Pórtico</v>
       </c>
       <c r="G22" s="26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Depois de 1983</v>
       </c>
       <c r="H22" s="26" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Betão Armado</v>
       </c>
       <c r="J22" s="55"/>
@@ -4135,15 +4135,15 @@
         <v>2.7027027027027029E-2</v>
       </c>
       <c r="O22" s="26" t="str">
-        <f t="shared" ref="O22:O24" si="27">VLOOKUP(L22,$S$1:$V$12,2,FALSE)</f>
+        <f t="shared" ref="O22:O24" si="28">VLOOKUP(L22,$S$1:$V$12,2,FALSE)</f>
         <v>Pórtico</v>
       </c>
       <c r="P22" s="26" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>Depois de 1983</v>
       </c>
       <c r="Q22" s="26" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -4164,15 +4164,15 @@
         <v>0.27272727272727271</v>
       </c>
       <c r="F23" s="26" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Tabuleiro simples/apoiado</v>
       </c>
       <c r="G23" s="26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Antes de 1983</v>
       </c>
       <c r="H23" s="26" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Betão Armado</v>
       </c>
       <c r="J23" s="55"/>
@@ -4191,15 +4191,15 @@
         <v>2.7027027027027029E-2</v>
       </c>
       <c r="O23" s="26" t="str">
+        <f t="shared" si="28"/>
+        <v>Tabuleiro simples/apoiado</v>
+      </c>
+      <c r="P23" s="26" t="str">
+        <f t="shared" si="26"/>
+        <v>Antes de 1983</v>
+      </c>
+      <c r="Q23" s="26" t="str">
         <f t="shared" si="27"/>
-        <v>Tabuleiro simples/apoiado</v>
-      </c>
-      <c r="P23" s="26" t="str">
-        <f t="shared" si="25"/>
-        <v>Antes de 1983</v>
-      </c>
-      <c r="Q23" s="26" t="str">
-        <f t="shared" si="26"/>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -4220,15 +4220,15 @@
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="F24" s="26" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Vãos Multiplos</v>
       </c>
       <c r="G24" s="26" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Depois de 1983</v>
       </c>
       <c r="H24" s="26" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Betão Armado</v>
       </c>
       <c r="J24" s="56"/>
@@ -4247,15 +4247,15 @@
         <v>0.91891891891891897</v>
       </c>
       <c r="O24" s="26" t="str">
+        <f t="shared" si="28"/>
+        <v>Vãos Multiplos</v>
+      </c>
+      <c r="P24" s="26" t="str">
+        <f t="shared" si="26"/>
+        <v>Depois de 1983</v>
+      </c>
+      <c r="Q24" s="26" t="str">
         <f t="shared" si="27"/>
-        <v>Vãos Multiplos</v>
-      </c>
-      <c r="P24" s="26" t="str">
-        <f t="shared" si="25"/>
-        <v>Depois de 1983</v>
-      </c>
-      <c r="Q24" s="26" t="str">
-        <f t="shared" si="26"/>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -4279,11 +4279,11 @@
         <v>Vãos Multiplos</v>
       </c>
       <c r="P26" s="25" t="str">
-        <f t="shared" ref="P26:P30" si="28">VLOOKUP(L26,$S$1:$V$12,3,FALSE)</f>
+        <f t="shared" ref="P26:P30" si="29">VLOOKUP(L26,$S$1:$V$12,3,FALSE)</f>
         <v>Depois de 1983</v>
       </c>
       <c r="Q26" s="25" t="str">
-        <f t="shared" ref="Q26:Q30" si="29">VLOOKUP(L26,$S$1:$V$12,4,FALSE)</f>
+        <f t="shared" ref="Q26:Q30" si="30">VLOOKUP(L26,$S$1:$V$12,4,FALSE)</f>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -4308,11 +4308,11 @@
         <v>0</v>
       </c>
       <c r="P27" s="26">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="Q27" s="26" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Alvenaria</v>
       </c>
     </row>
@@ -4333,15 +4333,15 @@
         <v>1.0050251256281407E-2</v>
       </c>
       <c r="O28" s="26" t="str">
-        <f t="shared" ref="O28:O30" si="30">VLOOKUP(L28,$S$1:$V$12,2,FALSE)</f>
+        <f t="shared" ref="O28:O30" si="31">VLOOKUP(L28,$S$1:$V$12,2,FALSE)</f>
         <v>Pórtico</v>
       </c>
       <c r="P28" s="26" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>Depois de 1983</v>
       </c>
       <c r="Q28" s="26" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -4362,15 +4362,15 @@
         <v>1.0050251256281407E-2</v>
       </c>
       <c r="O29" s="26" t="str">
+        <f t="shared" si="31"/>
+        <v>Tabuleiro simples/apoiado</v>
+      </c>
+      <c r="P29" s="26" t="str">
+        <f t="shared" si="29"/>
+        <v>Antes de 1983</v>
+      </c>
+      <c r="Q29" s="26" t="str">
         <f t="shared" si="30"/>
-        <v>Tabuleiro simples/apoiado</v>
-      </c>
-      <c r="P29" s="26" t="str">
-        <f t="shared" si="28"/>
-        <v>Antes de 1983</v>
-      </c>
-      <c r="Q29" s="26" t="str">
-        <f t="shared" si="29"/>
         <v>Betão Armado</v>
       </c>
     </row>
@@ -4391,31 +4391,31 @@
         <v>2.5125628140703518E-3</v>
       </c>
       <c r="O30" s="26" t="str">
+        <f t="shared" si="31"/>
+        <v>Tabuleiro simples/apoiado</v>
+      </c>
+      <c r="P30" s="26" t="str">
+        <f t="shared" si="29"/>
+        <v>Depois de 1983</v>
+      </c>
+      <c r="Q30" s="26" t="str">
         <f t="shared" si="30"/>
-        <v>Tabuleiro simples/apoiado</v>
-      </c>
-      <c r="P30" s="26" t="str">
-        <f t="shared" si="28"/>
-        <v>Depois de 1983</v>
-      </c>
-      <c r="Q30" s="26" t="str">
-        <f t="shared" si="29"/>
         <v>Betão Armado</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="J14:J18"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="J26:J30"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="J8:J12"/>
     <mergeCell ref="J20:J24"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="J14:J18"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4428,22 +4428,22 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:E12"/>
+      <selection pane="topRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.54296875" style="31" customWidth="1"/>
     <col min="7" max="7" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="105.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>